<commit_message>
update neues sensoren excel + drop non relevant entityid's
</commit_message>
<xml_diff>
--- a/Sensoren.xlsx
+++ b/Sensoren.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fschmidmichels\sciebo\DLO\Lehre\Business Intelligence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e055413514c2be64/Dokumente/!STUDIUM/5. Semester/Business Intelligence (BI)/70^1 Challenge/bi-70-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BA4B26DB-44DC-4DA3-95FD-E919BD1954B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38B9CECD-3E81-46E5-B0C3-D8CF33E5E35D}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="3495" windowWidth="24675" windowHeight="12120"/>
+    <workbookView xWindow="4110" yWindow="2145" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensoren" sheetId="1" r:id="rId1"/>
@@ -28,15 +29,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Abfrage - entities" description="Verbindung mit der Abfrage 'entities' in der Arbeitsmappe." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Abfrage - entities" description="Verbindung mit der Abfrage 'entities' in der Arbeitsmappe." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=entities;Extended Properties=&quot;&quot;" command="SELECT * FROM [entities]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="157">
   <si>
     <t>Sensor#1 Sensor Status</t>
   </si>
@@ -299,12 +300,6 @@
     <t>DHT 22 Temperature</t>
   </si>
   <si>
-    <t>SenseAir CO2 Value</t>
-  </si>
-  <si>
-    <t>sensor.senseair_co2_value</t>
-  </si>
-  <si>
     <t>Temperatur in Raum G013 (Laut Hersteller +- 0,5°C)</t>
   </si>
   <si>
@@ -416,9 +411,6 @@
     <t>Print Entities To File</t>
   </si>
   <si>
-    <t>ESP8266 + CCS811 für Messung von flüchtigen organischen Substanzen und indirekte Berechnung einen äquivalenten CO2 Werts + SenseAir S8 für Messung von CO2 Wert + DHT22 Sensor für Temperatur und Luftfeuchtigkeit</t>
-  </si>
-  <si>
     <t>ESP8266 + BME280 Chip für Luftfeuchtigkeit und Luftdruck und BH1750 für die Beleuchtungsstärke</t>
   </si>
   <si>
@@ -504,12 +496,24 @@
   </si>
   <si>
     <t>Steckdosenzwischenstecker mit WLAN, der diverse elektrische Messwerte liefert. Misst den Homeassistant, Fischer Technik, Laborrechner.</t>
+  </si>
+  <si>
+    <t>sensor.mh_z19_co2_value</t>
+  </si>
+  <si>
+    <t>MH-Z19 CO2 Value</t>
+  </si>
+  <si>
+    <t>ESP8266 + CCS811 für Messung von flüchtigen organischen Substanzen und indirekte Berechnung einen äquivalenten CO2 Werts + MH-Z19 Sensor für Messung von CO2 Wert + DHT22 Sensor für Temperatur und Luftfeuchtigkeit</t>
+  </si>
+  <si>
+    <t>Für eine genauere Beschreibung bitte die Tabelle entity_id lesen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,7 +581,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExterneDaten_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="6" unboundColumnsRight="1">
     <queryTableFields count="4">
       <queryTableField id="2" name="Column2" tableColumnId="8"/>
@@ -590,16 +594,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entities" displayName="entities" ref="A1:D53" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D53"/>
-  <sortState ref="A2:D53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="entities" displayName="entities" ref="A1:D53" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
     <sortCondition ref="B2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="8" uniqueName="8" name="entity_id" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="7" uniqueName="7" name="Sensorname / Beschreibung" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="9" uniqueName="9" name="Physikalische Einheit" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="10" uniqueName="10" name="Funktion" queryTableFieldId="5" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="entity_id" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Sensorname / Beschreibung" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Physikalische Einheit" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="Funktion" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -867,11 +871,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +888,7 @@
         <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,15 +904,15 @@
         <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -916,7 +920,12 @@
         <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -926,18 +935,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="82.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -961,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -975,7 +984,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -989,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1003,7 +1012,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -1017,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -1031,13 +1040,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,18 +1054,18 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>86</v>
@@ -1065,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
@@ -1099,7 +1108,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>55</v>
@@ -1113,7 +1122,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>55</v>
@@ -1127,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
@@ -1136,16 +1145,16 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,7 +1162,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
@@ -1181,7 +1190,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>22</v>
@@ -1195,7 +1204,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
@@ -1209,7 +1218,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -1223,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>55</v>
@@ -1237,7 +1246,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
@@ -1251,7 +1260,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>24</v>
@@ -1265,7 +1274,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>55</v>
@@ -1279,7 +1288,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>55</v>
@@ -1293,7 +1302,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>22</v>
@@ -1307,7 +1316,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
@@ -1318,13 +1327,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>81</v>
@@ -1332,10 +1341,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>34</v>
@@ -1346,13 +1355,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>66</v>
@@ -1360,10 +1369,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>38</v>
@@ -1374,13 +1383,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>67</v>
@@ -1388,10 +1397,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>42</v>
@@ -1402,10 +1411,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>42</v>
@@ -1416,10 +1425,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>45</v>
@@ -1430,10 +1439,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>47</v>
@@ -1444,10 +1453,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>42</v>
@@ -1458,10 +1467,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>45</v>
@@ -1475,7 +1484,7 @@
         <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>55</v>
@@ -1489,7 +1498,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -1506,7 +1515,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>34</v>
@@ -1523,7 +1532,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>36</v>
@@ -1540,7 +1549,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>38</v>
@@ -1554,7 +1563,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>40</v>
@@ -1568,7 +1577,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>42</v>
@@ -1582,7 +1591,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>42</v>
@@ -1596,7 +1605,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>45</v>
@@ -1610,7 +1619,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>47</v>
@@ -1624,7 +1633,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>42</v>
@@ -1638,7 +1647,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -1652,7 +1661,7 @@
         <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>55</v>
@@ -1666,7 +1675,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>55</v>
@@ -1680,7 +1689,7 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="2" t="s">

</xml_diff>